<commit_message>
update payment filtre date session
</commit_message>
<xml_diff>
--- a/public/assets-panel/course.xlsx
+++ b/public/assets-panel/course.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\LMSProject\public\assets-panel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C792E4B3-23EB-4622-8A1D-52F408548C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F27F29-9274-46EE-A06B-AF5A3F0958C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30705" yWindow="2850" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="870" yWindow="-120" windowWidth="23250" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>BODY</t>
   </si>
   <si>
-    <t>CATEGORY</t>
-  </si>
-  <si>
     <t xml:space="preserve">course java </t>
   </si>
   <si>
@@ -42,16 +39,22 @@
     <t>course java 2</t>
   </si>
   <si>
-    <t>Web</t>
-  </si>
-  <si>
-    <t>IOS</t>
-  </si>
-  <si>
     <t>ios</t>
   </si>
   <si>
     <t>TITLE</t>
+  </si>
+  <si>
+    <t>CATEGORY ID</t>
+  </si>
+  <si>
+    <t>SUB CATEGORY ID</t>
+  </si>
+  <si>
+    <t>TARGET ID</t>
+  </si>
+  <si>
+    <t>ID COMPANY</t>
   </si>
 </sst>
 </file>
@@ -369,48 +372,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>1.3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
+      <c r="F3">
+        <v>4.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>